<commit_message>
Completed Tests on Ranking
</commit_message>
<xml_diff>
--- a/Risultati/Risultati Search Engine.xlsx
+++ b/Risultati/Risultati Search Engine.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="1" r:id="rId1"/>
-    <sheet name="Matching Times" sheetId="2" r:id="rId2"/>
-    <sheet name="Queries" sheetId="3" r:id="rId3"/>
+    <sheet name="Queries" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>load graph</t>
   </si>
@@ -33,24 +32,12 @@
     <t>PageRank</t>
   </si>
   <si>
-    <t>PageRank parallel</t>
-  </si>
-  <si>
-    <t>HITS parallel</t>
-  </si>
-  <si>
     <t>VALORI IN MEDIA SU 10 Run</t>
   </si>
   <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Best Match</t>
-  </si>
-  <si>
-    <t>Improved best match</t>
-  </si>
-  <si>
     <t>Query 1</t>
   </si>
   <si>
@@ -81,9 +68,6 @@
     <t>Query 10</t>
   </si>
   <si>
-    <t>Query</t>
-  </si>
-  <si>
     <t>Lunghezza</t>
   </si>
   <si>
@@ -316,6 +300,15 @@
   </si>
   <si>
     <t>30000 (full)</t>
+  </si>
+  <si>
+    <t>HITS parallel 4 jobs</t>
+  </si>
+  <si>
+    <t>full , 10 iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HITS </t>
   </si>
 </sst>
 </file>
@@ -570,11 +563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="418500744"/>
-        <c:axId val="418503488"/>
+        <c:axId val="271060520"/>
+        <c:axId val="270204544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="418500744"/>
+        <c:axId val="271060520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -616,7 +609,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418503488"/>
+        <c:crossAx val="270204544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -624,7 +617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418503488"/>
+        <c:axId val="270204544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +667,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418500744"/>
+        <c:crossAx val="271060520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -817,7 +810,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>(Ranking!$B$2,Ranking!$B$4,Ranking!$B$6,Ranking!$B$8,Ranking!$B$10,Ranking!$B$12)</c:f>
+              <c:f>(Ranking!$B$3,Ranking!$B$5,Ranking!$B$7,Ranking!$B$9,Ranking!$B$11,Ranking!$B$13)</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -848,22 +841,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.156</c:v>
+                  <c:v>3.157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06</c:v>
+                  <c:v>8.6340000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95</c:v>
+                  <c:v>29.806000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.326000000000001</c:v>
+                  <c:v>77.531999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.635999999999999</c:v>
+                  <c:v>213.72499999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85.07</c:v>
+                  <c:v>427.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,11 +872,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="418497608"/>
-        <c:axId val="418498392"/>
+        <c:axId val="270473832"/>
+        <c:axId val="270474216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="418497608"/>
+        <c:axId val="270473832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +918,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418498392"/>
+        <c:crossAx val="270474216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -933,7 +926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="418498392"/>
+        <c:axId val="270474216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +976,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="418497608"/>
+        <c:crossAx val="270473832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1269,11 +1262,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="361510400"/>
-        <c:axId val="361511576"/>
+        <c:axId val="133916480"/>
+        <c:axId val="133916088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361510400"/>
+        <c:axId val="133916480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1308,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361511576"/>
+        <c:crossAx val="133916088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1323,7 +1316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361511576"/>
+        <c:axId val="133916088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1366,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361510400"/>
+        <c:crossAx val="133916480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1707,11 +1700,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="361505696"/>
-        <c:axId val="361508048"/>
+        <c:axId val="270653968"/>
+        <c:axId val="270651616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="361505696"/>
+        <c:axId val="270653968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1753,7 +1746,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361508048"/>
+        <c:crossAx val="270651616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1761,7 +1754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="361508048"/>
+        <c:axId val="270651616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,7 +1804,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361505696"/>
+        <c:crossAx val="270653968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4439,10 +4432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4464,7 +4457,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4484,7 +4477,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F11" si="0">SUM(C2:E2)</f>
+        <f t="shared" ref="F2:F13" si="0">SUM(C2:E2)</f>
         <v>16.150000000000002</v>
       </c>
     </row>
@@ -4496,17 +4489,17 @@
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D3">
-        <v>0.156</v>
+        <v>3.157</v>
       </c>
       <c r="E3">
-        <v>3.2000000000000001E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>0.20100000000000001</v>
+        <v>3.1999999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4538,17 +4531,17 @@
         <v>2000</v>
       </c>
       <c r="C5">
-        <v>2.8000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D5">
-        <v>2.06</v>
+        <v>8.6340000000000003</v>
       </c>
       <c r="E5">
-        <v>0.06</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>2.1480000000000001</v>
+        <v>8.7219999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4580,17 +4573,17 @@
         <v>5000</v>
       </c>
       <c r="C7">
-        <v>8.2000000000000003E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D7">
-        <v>0.95</v>
+        <v>29.806000000000001</v>
       </c>
       <c r="E7">
-        <v>0.16200000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>1.194</v>
+        <v>30.024000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4622,17 +4615,17 @@
         <v>10000</v>
       </c>
       <c r="C9">
-        <v>0.17699999999999999</v>
+        <v>0.183</v>
       </c>
       <c r="D9">
-        <v>10.326000000000001</v>
+        <v>77.531999999999996</v>
       </c>
       <c r="E9">
-        <v>0.308</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>10.811</v>
+        <v>78.007000000000005</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4664,17 +4657,17 @@
         <v>20000</v>
       </c>
       <c r="C11">
-        <v>0.46700000000000003</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="D11">
-        <v>24.635999999999999</v>
+        <v>213.72499999999999</v>
       </c>
       <c r="E11">
-        <v>0.628</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>25.730999999999998</v>
+        <v>214.75199999999998</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4682,7 +4675,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C12">
         <v>4.9000000000000004</v>
@@ -4694,7 +4687,7 @@
         <v>0.33</v>
       </c>
       <c r="F12">
-        <f>SUM(C12:E12)</f>
+        <f t="shared" si="0"/>
         <v>5.33</v>
       </c>
     </row>
@@ -4703,35 +4696,46 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C13">
-        <v>0.79</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="D13">
-        <v>85.07</v>
+        <v>427.68</v>
       </c>
       <c r="E13">
-        <v>0.9</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="F13">
-        <f>SUM(C13:E13)</f>
-        <v>86.76</v>
+        <f t="shared" si="0"/>
+        <v>429.56900000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27">
+        <v>53.41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28">
+        <v>4.1500000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -4743,169 +4747,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-      <c r="Z1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="Z4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AQ16" sqref="AQ16"/>
     </sheetView>
   </sheetViews>
@@ -4922,39 +4766,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2">
         <v>1.6000000000000001E-3</v>
@@ -4967,24 +4811,24 @@
         <v>1.0000000000000005E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <v>2.0000000000000001E-4</v>
@@ -4997,24 +4841,24 @@
         <v>1E-4</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001E-3</v>
@@ -5027,24 +4871,24 @@
         <v>-8.9999999999999998E-4</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5">
         <v>3.0000000000000001E-3</v>
@@ -5057,27 +4901,27 @@
         <v>2E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D6">
         <v>4.0000000000000002E-4</v>
@@ -5090,19 +4934,19 @@
         <v>3.0000000000000003E-4</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D7" s="6">
         <f>AVERAGE(D2:D6)</f>
@@ -5119,13 +4963,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>8.9999999999999993E-3</v>
@@ -5138,24 +4982,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>2E-3</v>
@@ -5168,24 +5012,24 @@
         <v>1.6000000000000001E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <v>4.0000000000000001E-3</v>
@@ -5198,24 +5042,24 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D11">
         <v>2E-3</v>
@@ -5228,24 +5072,24 @@
         <v>1.7000000000000001E-3</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D12">
         <v>4.0000000000000001E-3</v>
@@ -5258,19 +5102,19 @@
         <v>1E-3</v>
       </c>
       <c r="G12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="C13" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D13" s="6">
         <f>AVERAGE(D8:D12)</f>
@@ -5287,13 +5131,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>0.01</v>
@@ -5306,24 +5150,24 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>1E-4</v>
@@ -5336,24 +5180,24 @@
         <v>-3.0000000000000003E-4</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>2E-3</v>
@@ -5366,24 +5210,24 @@
         <v>1.4000000000000002E-3</v>
       </c>
       <c r="G16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D17">
         <v>6.9999999999999999E-4</v>
@@ -5396,24 +5240,24 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D18">
         <v>2E-3</v>
@@ -5426,19 +5270,19 @@
         <v>1E-3</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="C19" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D19" s="6">
         <f>AVERAGE(D14:D18)</f>
@@ -5455,13 +5299,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D20">
         <v>2.5999999999999999E-3</v>
@@ -5474,24 +5318,24 @@
         <v>2.0000000000000009E-4</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>2E-3</v>
@@ -5504,24 +5348,24 @@
         <v>-1E-3</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D22">
         <v>1.2999999999999999E-2</v>
@@ -5534,24 +5378,24 @@
         <v>-2.2000000000000006E-2</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D23">
         <v>1.1999999999999999E-3</v>
@@ -5564,24 +5408,24 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I23" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D24">
         <v>3.5000000000000001E-3</v>
@@ -5594,19 +5438,19 @@
         <v>-2.9999999999999992E-4</v>
       </c>
       <c r="G24" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
       <c r="C25" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D25" s="6">
         <f>AVERAGE(D20:D24)</f>
@@ -5623,13 +5467,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D26">
         <v>1.2E-2</v>
@@ -5642,24 +5486,24 @@
         <v>-1.7999999999999999E-2</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H26" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>0.01</v>
@@ -5672,24 +5516,24 @@
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="G27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I27" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D28">
         <v>6.0000000000000001E-3</v>
@@ -5702,24 +5546,24 @@
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D29">
         <v>1.2999999999999999E-3</v>
@@ -5732,24 +5576,24 @@
         <v>1.0000000000000005E-4</v>
       </c>
       <c r="G29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I29" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D30">
         <v>0.01</v>
@@ -5762,19 +5606,19 @@
         <v>-2E-3</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
       <c r="C31" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D31" s="6">
         <f>AVERAGE(D26:D30)</f>

</xml_diff>

<commit_message>
Saving results and starting to prepare formal presentation of them
</commit_message>
<xml_diff>
--- a/Risultati/Risultati Search Engine.xlsx
+++ b/Risultati/Risultati Search Engine.xlsx
@@ -4,18 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="1" r:id="rId1"/>
     <sheet name="Queries" sheetId="3" r:id="rId2"/>
+    <sheet name="Query " sheetId="4" r:id="rId3"/>
+    <sheet name="Query  " sheetId="6" r:id="rId4"/>
+    <sheet name="Query  11" sheetId="7" r:id="rId5"/>
+    <sheet name="Query  (4)" sheetId="8" r:id="rId6"/>
+    <sheet name="Query  21" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>load graph</t>
   </si>
@@ -134,168 +139,12 @@
     <t>Trovato in IMP BS?</t>
   </si>
   <si>
-    <t>islands republic saint united south new island</t>
-  </si>
-  <si>
-    <t>http://www.lonelyplanet.com/blog/2014/05/01/meet-a-traveller-bruce-poon-tip-founder-of-g-adventures/</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>enterprise university building 906-487-4318 722 room</t>
-  </si>
-  <si>
-    <t>http://www.mtu.edu/enterprise/</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>nasa research 101</t>
-  </si>
-  <si>
-    <t>http://www.nasa.gov/centers/ames/home/directions.html</t>
-  </si>
-  <si>
-    <t>rights lucasfilm 2011 part tm</t>
-  </si>
-  <si>
-    <t>http://www.cartoonnetwork.com/tv_shows/adventuretime/characters/fionna/index.html</t>
-  </si>
-  <si>
-    <t>astro camp stennis space activities education</t>
-  </si>
-  <si>
-    <t>http://www.nasa.gov/offices/education/programs/descriptions/Astro_Camp.html</t>
-  </si>
-  <si>
-    <t>firstmerit bank 7th</t>
-  </si>
-  <si>
-    <t>http://www.mtu.edu/giving/ways-to-give/annual-gift/</t>
-  </si>
-  <si>
-    <t>actor towboy midnight factotum matt</t>
-  </si>
-  <si>
-    <t>http://www.ign.com/stars/matt-dillon</t>
-  </si>
-  <si>
-    <t>politics defense home senate</t>
-  </si>
-  <si>
     <t>BS-IMP</t>
   </si>
   <si>
-    <t>http://www.foxnews.com/politics/2014/06/02/three-cops-in-new-mexicos-infamous-anal-cavity-search-case-still-on-job/?intcmp=latestnews</t>
-  </si>
-  <si>
-    <t>may pdt 2014 30 ago hours</t>
-  </si>
-  <si>
-    <t>http://www.imdb.com/news/ns0000344/?ref_=hm_nw_tv_t4</t>
-  </si>
-  <si>
-    <t>rated rate stars</t>
-  </si>
-  <si>
-    <t>http://www.imdb.com/title/tt2364975/?ref_=inth_ov_tt</t>
-  </si>
-  <si>
-    <t>national park islands republic saint collection now</t>
-  </si>
-  <si>
-    <t>http://www.lonelyplanet.com/usa/yosemite-national-park</t>
-  </si>
-  <si>
-    <t>movies mini wars star movie filter-movies episode</t>
-  </si>
-  <si>
-    <t>http://www.lego.com/en-us/starwars/movies/movies/s4c5-bad</t>
-  </si>
-  <si>
-    <t>leadspace styles call 1-866-426-4252 us</t>
-  </si>
-  <si>
-    <t>http://www.ibm.com/smarterplanet/us/en/business_resilience_management/nextsteps/</t>
-  </si>
-  <si>
-    <t>islands republic seville</t>
-  </si>
-  <si>
-    <t>http://www.lonelyplanet.com/spain/seville/things-to-do/best-places-to-eat-in-seville</t>
-  </si>
-  <si>
-    <t>probabilmente island ha alto impatto</t>
-  </si>
-  <si>
-    <t>styles leadspace neck solutions specialized</t>
-  </si>
-  <si>
-    <t>http://www.ibm.com/smarterplanet/us/en/retail_analytics/examples/</t>
-  </si>
-  <si>
-    <t>movies mini wars star</t>
-  </si>
-  <si>
-    <t>http://www.lego.com/en-us/starwars/movies/commercials</t>
-  </si>
-  <si>
-    <t>arts performing visual keweenaw orchestra oct 730</t>
-  </si>
-  <si>
-    <t>http://www.mtu.edu/vpa/events/13-14/kso-color/</t>
-  </si>
-  <si>
-    <t>soccer cartoon rights superstar turner 2011 choose</t>
-  </si>
-  <si>
-    <t>http://www.cartoonnetwork.com/games/cc/superstar-soccer/index.html?atclk_hp=hpg_Games_Cartoon-Network_Superstar-Soccer</t>
-  </si>
-  <si>
-    <t>aqua mission page data</t>
-  </si>
-  <si>
-    <t>http://www.nasa.gov/mission_pages/aqua/</t>
-  </si>
-  <si>
-    <t>screen favorite cartoon network</t>
-  </si>
-  <si>
-    <t>http://www.cartoonnetwork.com/tv_shows/redakai/video/index.html</t>
-  </si>
-  <si>
-    <t>alumni tech michigan donald</t>
-  </si>
-  <si>
-    <t>http://www.mtu.edu/alumni/notables/profiles/Donald-Daavettila.html</t>
-  </si>
-  <si>
-    <t>sciences rich keweenaw</t>
-  </si>
-  <si>
-    <t>http://www.mtu.edu/social-sciences/undergraduate/history/</t>
-  </si>
-  <si>
-    <t>faculty student teams research will</t>
-  </si>
-  <si>
-    <t>http://www.nasa.gov/offices/education/programs/descriptions/Faculty_Student_Teams_Project.html</t>
-  </si>
-  <si>
-    <t>asking millennials hitman turns president takes</t>
-  </si>
-  <si>
-    <t>http://www.foxnews.com/on-air/happening-now/blog/2013/07/19/friday-july-19-2013-happening-now-detroit-bankrupt-us-baking</t>
-  </si>
-  <si>
-    <t>race vehicles great car take twistiest</t>
-  </si>
-  <si>
-    <t>http://www.lego.com/en-us/city/products/great-vehicles/60053-race-car</t>
-  </si>
-  <si>
     <t>MEDIA</t>
   </si>
   <si>
@@ -309,6 +158,126 @@
   </si>
   <si>
     <t xml:space="preserve">HITS </t>
+  </si>
+  <si>
+    <t>QUERY</t>
+  </si>
+  <si>
+    <t>BEST MATCH</t>
+  </si>
+  <si>
+    <t>PAGERANK</t>
+  </si>
+  <si>
+    <t>HITS authority</t>
+  </si>
+  <si>
+    <t>IMPROVED BEST MATCH</t>
+  </si>
+  <si>
+    <t>LENGTH</t>
+  </si>
+  <si>
+    <t>EXPECTED LINK</t>
+  </si>
+  <si>
+    <t>FOUND IN BS?</t>
+  </si>
+  <si>
+    <t>FOUND IN IBS?</t>
+  </si>
+  <si>
+    <t>The Duty Call Advanced Warfare</t>
+  </si>
+  <si>
+    <t>TEMPO BS</t>
+  </si>
+  <si>
+    <t>TEMPO IBS</t>
+  </si>
+  <si>
+    <t>http://www.ign.com/wikis/call-of-duty-advanced-warfare?objectid=20017429</t>
+  </si>
+  <si>
+    <t>http://www.ibm.com/connect/ibm/us/en/index.html</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>mortal combat wiki</t>
+  </si>
+  <si>
+    <t>UN resolution climate change</t>
+  </si>
+  <si>
+    <t>michael jordan nba basket matches</t>
+  </si>
+  <si>
+    <t>lego star wars clone republica cannon</t>
+  </si>
+  <si>
+    <t>space station The will It This first</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/forkids/kidsclub/text/Phase_6_Putting_It_All_Together.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/forstudents/k-4/stories/what-is-the-iss-k4.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/forstudents/5-8/features/what-is-the-iss-58.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/foreducators/expeditions/stem/stem-math-index.html</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/juniors/games/firetruck</t>
+  </si>
+  <si>
+    <t>http://www.un.org/en/documents/contact.asp</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/juniors/games/gas-station</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/juniors/games/gas-station?icmp=COUSGamesGLJuniorsGasStation</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/forstudents/k-4/stories/what-is-orion-k4.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/forstudents/k-4/stories/what-is-juno-k4.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/foreducators/teachingfromspace/dayinthelife/index.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/audience/foreducators/expeditions/stem/stem-tech-index.html</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/juniors/games/pony?icmp=COUSGamesGLJuniorsPony</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/juniors/games/pony</t>
+  </si>
+  <si>
+    <t>http://www.lego.com/en-us/city/codepage</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/mission_pages/station/research/index.html</t>
+  </si>
+  <si>
+    <t>http://www.nasa.gov/about/highlights/AN_Structure_OtherAgencies.html</t>
+  </si>
+  <si>
+    <t>http://www.ign.com/wikis/halo-master-chief-collection</t>
+  </si>
+  <si>
+    <t>http://www.ign.com/wikis/halo-master-chief-collection?save=successful</t>
+  </si>
+  <si>
+    <t>http://www.ign.com/articles/2014/06/05/earthnight-coming-to-ps4-ps-vita</t>
   </si>
 </sst>
 </file>
@@ -376,7 +345,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -384,12 +353,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -400,6 +384,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -602,11 +589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302785600"/>
-        <c:axId val="302785984"/>
+        <c:axId val="107046616"/>
+        <c:axId val="107047008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302785600"/>
+        <c:axId val="107046616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +635,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302785984"/>
+        <c:crossAx val="107047008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -656,7 +643,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302785984"/>
+        <c:axId val="107047008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +693,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302785600"/>
+        <c:crossAx val="107046616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -942,11 +929,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302042048"/>
-        <c:axId val="302041656"/>
+        <c:axId val="108494224"/>
+        <c:axId val="108496184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302042048"/>
+        <c:axId val="108494224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +975,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302041656"/>
+        <c:crossAx val="108496184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -996,7 +983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302041656"/>
+        <c:axId val="108496184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1033,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302042048"/>
+        <c:crossAx val="108494224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1254,19 +1241,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2600000000000003E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2000000000000006E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.96E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4599999999999996E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8599999999999989E-3</c:v>
+                  <c:v>0.47318601608299998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1304,19 +1291,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.4000000000000008E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.14E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4000000000000014E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9600000000000009E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3439999999999999E-2</c:v>
+                  <c:v>1.6916990280199998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1332,11 +1319,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="302043224"/>
-        <c:axId val="302043616"/>
+        <c:axId val="108494616"/>
+        <c:axId val="108496968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="302043224"/>
+        <c:axId val="108494616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,7 +1365,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302043616"/>
+        <c:crossAx val="108496968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1386,7 +1373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="302043616"/>
+        <c:axId val="108496968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,7 +1423,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="302043224"/>
+        <c:crossAx val="108494616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1681,19 +1668,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.2600000000000003E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2000000000000006E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.96E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.4599999999999996E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8599999999999989E-3</c:v>
+                  <c:v>0.47318601608299998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,19 +1729,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9.4000000000000008E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.14E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.4000000000000014E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9600000000000009E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3439999999999999E-2</c:v>
+                  <c:v>1.6916990280199998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,11 +1757,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="303579584"/>
-        <c:axId val="303574880"/>
+        <c:axId val="108495400"/>
+        <c:axId val="108498928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="303579584"/>
+        <c:axId val="108495400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1803,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303574880"/>
+        <c:crossAx val="108498928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1824,7 +1811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="303574880"/>
+        <c:axId val="108498928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1874,7 +1861,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="303579584"/>
+        <c:crossAx val="108495400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4504,7 +4491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="N2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -4745,7 +4732,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>4.9000000000000004</v>
@@ -4766,7 +4753,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>0.98099999999999998</v>
@@ -4789,12 +4776,12 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>53.41</v>
@@ -4802,7 +4789,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="B28">
         <v>4.1500000000000004</v>
@@ -4819,8 +4806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AQ16" sqref="AQ16"/>
+    <sheetView topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4832,6 +4819,7 @@
     <col min="7" max="7" width="25.140625" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="47" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -4848,7 +4836,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
@@ -4858,6 +4846,9 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4868,26 +4859,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="E2">
-        <v>1.5E-3</v>
-      </c>
-      <c r="F2">
-        <f>D2-E2</f>
-        <v>1.0000000000000005E-4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4897,28 +4869,6 @@
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="E3">
-        <v>1E-4</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F30" si="0">D3-E3</f>
-        <v>1E-4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -4927,28 +4877,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="E4">
-        <v>2E-3</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>-8.9999999999999998E-4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -4957,31 +4886,6 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E5">
-        <v>1E-3</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>2E-3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -4990,45 +4894,23 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="E6">
-        <v>1E-4</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000003E-4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="7" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="6">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6" t="e">
         <f>AVERAGE(D2:D6)</f>
-        <v>1.2600000000000003E-3</v>
-      </c>
-      <c r="E7" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7" s="6" t="e">
         <f>AVERAGE(E2:E6)</f>
-        <v>9.4000000000000008E-4</v>
-      </c>
-      <c r="F7" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="6" t="e">
         <f>AVERAGE(F2:F6)</f>
-        <v>3.2000000000000008E-4</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5039,26 +4921,11 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="E8">
-        <v>1E-3</v>
+        <v>62</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
+        <f>D8-E8</f>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5068,27 +4935,9 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9">
-        <v>2E-3</v>
-      </c>
-      <c r="E9">
-        <v>4.0000000000000002E-4</v>
-      </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="G9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" t="s">
-        <v>41</v>
+        <f t="shared" ref="F3:F30" si="0">D9-E9</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5098,27 +4947,9 @@
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E10">
-        <v>1E-3</v>
-      </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5128,27 +4959,9 @@
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11">
-        <v>2E-3</v>
-      </c>
-      <c r="E11">
-        <v>2.9999999999999997E-4</v>
-      </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>1.7000000000000001E-3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5158,45 +4971,27 @@
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E12">
-        <v>3.0000000000000001E-3</v>
-      </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>82</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="C13" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="6">
+        <v>41</v>
+      </c>
+      <c r="D13" s="6" t="e">
         <f>AVERAGE(D8:D12)</f>
-        <v>4.2000000000000006E-3</v>
-      </c>
-      <c r="E13" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="6" t="e">
         <f>AVERAGE(E8:E12)</f>
-        <v>1.14E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F13" s="6">
         <f>AVERAGE(F8:F12)</f>
-        <v>3.0600000000000002E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5207,27 +5002,9 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14">
-        <v>0.01</v>
-      </c>
-      <c r="E14">
-        <v>2E-3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
-      <c r="I14" t="s">
-        <v>41</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -5236,28 +5013,6 @@
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15">
-        <v>1E-4</v>
-      </c>
-      <c r="E15">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>-3.0000000000000003E-4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -5266,28 +5021,6 @@
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16">
-        <v>2E-3</v>
-      </c>
-      <c r="E16">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>1.4000000000000002E-3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -5296,28 +5029,6 @@
       <c r="B17">
         <v>5</v>
       </c>
-      <c r="C17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D17">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="E17">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G17" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -5326,45 +5037,23 @@
       <c r="B18">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18">
-        <v>2E-3</v>
-      </c>
-      <c r="E18">
-        <v>1E-3</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-      <c r="G18" t="s">
-        <v>88</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="C19" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D19" s="6">
+        <v>41</v>
+      </c>
+      <c r="D19" s="6" t="e">
         <f>AVERAGE(D14:D18)</f>
-        <v>2.96E-3</v>
-      </c>
-      <c r="E19" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="6" t="e">
         <f>AVERAGE(E14:E18)</f>
-        <v>8.4000000000000014E-4</v>
-      </c>
-      <c r="F19" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="6" t="e">
         <f>AVERAGE(F14:F18)</f>
-        <v>2.1200000000000004E-3</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -5375,26 +5064,11 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="E20">
-        <v>2.3999999999999998E-3</v>
+        <v>64</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>2.0000000000000009E-4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -5404,27 +5078,9 @@
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21">
-        <v>2E-3</v>
-      </c>
-      <c r="E21">
-        <v>3.0000000000000001E-3</v>
-      </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>-1E-3</v>
-      </c>
-      <c r="G21" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -5434,27 +5090,9 @@
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E22">
-        <v>3.5000000000000003E-2</v>
-      </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>-2.2000000000000006E-2</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -5464,27 +5102,10 @@
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="E23">
-        <v>5.9999999999999995E-4</v>
-      </c>
+      <c r="C23" s="4"/>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="G23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" t="s">
-        <v>44</v>
-      </c>
-      <c r="I23" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -5494,45 +5115,27 @@
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="E24">
-        <v>3.8E-3</v>
-      </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>-2.9999999999999992E-4</v>
-      </c>
-      <c r="G24" t="s">
-        <v>92</v>
-      </c>
-      <c r="H24" t="s">
-        <v>44</v>
-      </c>
-      <c r="I24" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
       <c r="C25" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="6">
+        <v>41</v>
+      </c>
+      <c r="D25" s="6" t="e">
         <f>AVERAGE(D20:D24)</f>
-        <v>4.4599999999999996E-3</v>
-      </c>
-      <c r="E25" s="6">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E25" s="6" t="e">
         <f>AVERAGE(E20:E24)</f>
-        <v>8.9600000000000009E-3</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F25" s="6">
         <f>AVERAGE(F20:F24)</f>
-        <v>-4.5000000000000014E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5543,26 +5146,26 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>1.2E-2</v>
+        <v>0.47318601608299998</v>
       </c>
       <c r="E26">
-        <v>0.03</v>
+        <v>1.6916990280199998E-2</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>-1.7999999999999999E-2</v>
+        <v>0.45626902580279999</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -5572,27 +5175,9 @@
       <c r="B27">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27">
-        <v>0.01</v>
-      </c>
-      <c r="E27">
-        <v>1.4E-2</v>
-      </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>-4.0000000000000001E-3</v>
-      </c>
-      <c r="G27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -5602,27 +5187,10 @@
       <c r="B28">
         <v>7</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E28">
-        <v>0.01</v>
-      </c>
+      <c r="C28" s="3"/>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>-4.0000000000000001E-3</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" t="s">
-        <v>44</v>
-      </c>
-      <c r="I28" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -5632,27 +5200,9 @@
       <c r="B29">
         <v>7</v>
       </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="E29">
-        <v>1.1999999999999999E-3</v>
-      </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>1.0000000000000005E-4</v>
-      </c>
-      <c r="G29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I29" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -5662,59 +5212,1281 @@
       <c r="B30">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30">
-        <v>0.01</v>
-      </c>
-      <c r="E30">
-        <v>1.2E-2</v>
-      </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>-2E-3</v>
-      </c>
-      <c r="G30" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" t="s">
-        <v>44</v>
-      </c>
-      <c r="I30" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
       <c r="C31" s="6" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="D31" s="6">
         <f>AVERAGE(D26:D30)</f>
-        <v>7.8599999999999989E-3</v>
+        <v>0.47318601608299998</v>
       </c>
       <c r="E31" s="6">
         <f>AVERAGE(E26:E30)</f>
-        <v>1.3439999999999999E-2</v>
+        <v>1.6916990280199998E-2</v>
       </c>
       <c r="F31" s="6">
         <f>AVERAGE(F26:F30)</f>
-        <v>-5.5799999999999999E-3</v>
+        <v>9.1253805160560003E-2</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="F32" s="6">
+      <c r="F32" s="6" t="e">
         <f>AVERAGE(F7,F13,F19,F25,F31)</f>
-        <v>-9.1600000000000015E-4</v>
-      </c>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="69.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2">
+        <v>0.22014403343200001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1.22451903405899E-5</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.30730858148743E-5</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="10">
+        <v>5.1931818181818101E-6</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="10">
+        <v>5.4721664168040596E-6</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="10">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1.20452448760635E-5</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="10">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1.8452363336314102E-5</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1.7359516528926399E-5</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1.9402476155750199E-5</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2.54689697393084E-5</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1.2370595785032599E-8</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="10">
+        <v>5.4721664168040596E-6</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="10">
+        <v>1.8452363336314102E-5</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="10">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="10">
+        <v>5.1241264671323601E-5</v>
+      </c>
+      <c r="C21" s="10">
+        <v>5.5544105523551599E-7</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="10">
+        <v>5.43748836873962E-6</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="10">
+        <v>5.1469215394822304E-6</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="10">
+        <v>4.3494635989035301E-5</v>
+      </c>
+      <c r="C24" s="10">
+        <v>1.20476216749328E-6</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="10">
+        <v>9.0625332665379805E-6</v>
+      </c>
+      <c r="C25" s="10">
+        <v>5.4873559636968102E-8</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="10">
+        <v>8.3622676310891896E-6</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1.04063454274664E-7</v>
+      </c>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G14" r:id="rId1"/>
+    <hyperlink ref="A25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bugs, please stop happening
</commit_message>
<xml_diff>
--- a/Risultati/Risultati Search Engine.xlsx
+++ b/Risultati/Risultati Search Engine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Ranking" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
-  <si>
-    <t>load graph</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>HITS</t>
   </si>
   <si>
-    <t>dumping</t>
-  </si>
-  <si>
     <t>algorithm execution</t>
   </si>
   <si>
@@ -40,9 +34,6 @@
     <t>VALORI IN MEDIA SU 10 Run</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>Query 1</t>
   </si>
   <si>
@@ -76,12 +67,6 @@
     <t>Lunghezza</t>
   </si>
   <si>
-    <t>Testo</t>
-  </si>
-  <si>
-    <t>Documento atteso</t>
-  </si>
-  <si>
     <t>Query 11</t>
   </si>
   <si>
@@ -127,21 +112,12 @@
     <t>Query 25</t>
   </si>
   <si>
-    <t>Trovato in BS?</t>
-  </si>
-  <si>
     <t>Tempo BS</t>
   </si>
   <si>
     <t>Tempo IMP BS</t>
   </si>
   <si>
-    <t>Trovato in IMP BS?</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>BS-IMP</t>
   </si>
   <si>
@@ -200,21 +176,6 @@
   </si>
   <si>
     <t>http://www.ibm.com/connect/ibm/us/en/index.html</t>
-  </si>
-  <si>
-    <t>NOTE</t>
-  </si>
-  <si>
-    <t>mortal combat wiki</t>
-  </si>
-  <si>
-    <t>UN resolution climate change</t>
-  </si>
-  <si>
-    <t>michael jordan nba basket matches</t>
-  </si>
-  <si>
-    <t>lego star wars clone republica cannon</t>
   </si>
   <si>
     <t>space station The will It This first</t>
@@ -284,7 +245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,12 +272,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -380,13 +335,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -553,27 +508,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Ranking!$D$2,Ranking!$D$4,Ranking!$D$6,Ranking!$D$8,Ranking!$D$10,Ranking!$D$12)</c:f>
+              <c:f>(Ranking!$C$2,Ranking!$C$4,Ranking!$C$6,Ranking!$C$8,Ranking!$C$10,Ranking!$C$12)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>1.2053113041320101E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>3.1270832565536401E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4999999999999999E-2</c:v>
+                  <c:v>0.14399963798861601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>0.55848499168913301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2999999999999995E-2</c:v>
+                  <c:v>3.0424219494592899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1</c:v>
+                  <c:v>10.2829727759042</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,11 +544,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="107046616"/>
-        <c:axId val="107047008"/>
+        <c:axId val="305274416"/>
+        <c:axId val="140539000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107046616"/>
+        <c:axId val="305274416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +590,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107047008"/>
+        <c:crossAx val="140539000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -643,7 +598,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107047008"/>
+        <c:axId val="140539000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -693,7 +648,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107046616"/>
+        <c:crossAx val="305274416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -893,7 +848,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Ranking!$D$3,Ranking!$D$5,Ranking!$D$7,Ranking!$D$9,Ranking!$D$11,Ranking!$D$13)</c:f>
+              <c:f>(Ranking!$C$3,Ranking!$C$5,Ranking!$C$7,Ranking!$C$9,Ranking!$C$11,Ranking!$C$13)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -929,11 +884,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="108494224"/>
-        <c:axId val="108496184"/>
+        <c:axId val="140542136"/>
+        <c:axId val="140540176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108494224"/>
+        <c:axId val="140542136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +930,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108496184"/>
+        <c:crossAx val="140540176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -983,7 +938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108496184"/>
+        <c:axId val="140540176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1033,7 +988,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108494224"/>
+        <c:crossAx val="140542136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1134,13 +1089,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Tempi</a:t>
+              <a:t>Execution Times</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
-              <a:t> di esecuzione</a:t>
-            </a:r>
-            <a:endParaRPr lang="it-IT" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1236,24 +1186,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Queries!$D$7,Queries!$D$13,Queries!$D$19,Queries!$D$25,Queries!$D$31)</c:f>
+              <c:f>(Queries!$C$7,Queries!$C$13,Queries!$C$19,Queries!$C$25,Queries!$C$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.4906435012784998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21140398979177402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8.9908361435018E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.48650479316771006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47318601608299998</c:v>
+                  <c:v>0.74424324035627998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,24 +1236,24 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>(Queries!$E$7,Queries!$E$13,Queries!$E$19,Queries!$E$25,Queries!$E$31)</c:f>
+              <c:f>(Queries!$D$7,Queries!$D$13,Queries!$D$19,Queries!$D$25,Queries!$D$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.9952774047856002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.1078319549594008E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.1033744812040002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.9214611053469996E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6916990280199998E-2</c:v>
+                  <c:v>8.589172363273001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,11 +1269,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="108494616"/>
-        <c:axId val="108496968"/>
+        <c:axId val="140543704"/>
+        <c:axId val="140541352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108494616"/>
+        <c:axId val="140543704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1365,7 +1315,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108496968"/>
+        <c:crossAx val="140541352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1373,7 +1323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108496968"/>
+        <c:axId val="140541352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1373,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108494616"/>
+        <c:crossAx val="140543704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,8 +1505,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT" sz="2400"/>
-              <a:t>Proiezione esponenziale dei tempi</a:t>
+              <a:t>Exp(Execution</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" sz="2400" baseline="0"/>
+              <a:t> Times)</a:t>
+            </a:r>
+            <a:endParaRPr lang="it-IT" sz="2400"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1663,24 +1618,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Queries!$D$7,Queries!$D$13,Queries!$D$19,Queries!$D$25,Queries!$D$31)</c:f>
+              <c:f>(Queries!$C$7,Queries!$C$13,Queries!$C$19,Queries!$C$25,Queries!$C$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.4906435012784998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.21140398979177402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8.9908361435018E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.48650479316771006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47318601608299998</c:v>
+                  <c:v>0.74424324035627998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,24 +1679,24 @@
           </c:trendline>
           <c:val>
             <c:numRef>
-              <c:f>(Queries!$E$7,Queries!$E$13,Queries!$E$19,Queries!$E$25,Queries!$E$31)</c:f>
+              <c:f>(Queries!$D$7,Queries!$D$13,Queries!$D$19,Queries!$D$25,Queries!$D$31)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.9952774047856002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.1078319549594008E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.1033744812040002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.9214611053469996E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6916990280199998E-2</c:v>
+                  <c:v>8.589172363273001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1757,11 +1712,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="108495400"/>
-        <c:axId val="108498928"/>
+        <c:axId val="140537824"/>
+        <c:axId val="140540568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="108495400"/>
+        <c:axId val="140537824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1803,7 +1758,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108498928"/>
+        <c:crossAx val="140540568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1811,7 +1766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108498928"/>
+        <c:axId val="140540568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1861,7 +1816,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108495400"/>
+        <c:crossAx val="140537824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4074,13 +4029,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>19049</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>600074</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -4104,13 +4059,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4139,13 +4094,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>28574</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
@@ -4169,13 +4124,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
@@ -4489,299 +4444,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>1000</v>
       </c>
       <c r="C2">
-        <v>16.14</v>
-      </c>
-      <c r="D2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F13" si="0">SUM(C2:E2)</f>
-        <v>16.150000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.2053113041320101E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3">
-        <v>1.4E-2</v>
-      </c>
-      <c r="D3">
         <v>3.157</v>
       </c>
-      <c r="E3">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>3.1999999999999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2000</v>
       </c>
       <c r="C4">
-        <v>5.39</v>
-      </c>
-      <c r="D4">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="E4">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>5.4239999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.1270832565536401E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>2000</v>
       </c>
       <c r="C5">
-        <v>0.03</v>
-      </c>
-      <c r="D5">
         <v>8.6340000000000003</v>
       </c>
-      <c r="E5">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>8.7219999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>5000</v>
       </c>
       <c r="C6">
-        <v>5.19</v>
-      </c>
-      <c r="D6">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E6">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>5.2709999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.14399963798861601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>5000</v>
       </c>
       <c r="C7">
-        <v>7.8E-2</v>
-      </c>
-      <c r="D7">
         <v>29.806000000000001</v>
       </c>
-      <c r="E7">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>30.024000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>10000</v>
       </c>
       <c r="C8">
-        <v>5.45</v>
-      </c>
-      <c r="D8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="E8">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>5.6180000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.55848499168913301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>10000</v>
       </c>
       <c r="C9">
-        <v>0.183</v>
-      </c>
-      <c r="D9">
         <v>77.531999999999996</v>
       </c>
-      <c r="E9">
-        <v>0.29199999999999998</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>78.007000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>20000</v>
       </c>
       <c r="C10">
-        <v>5.37</v>
-      </c>
-      <c r="D10">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="E10">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>5.7060000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0424219494592899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>20000</v>
       </c>
       <c r="C11">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="D11">
         <v>213.72499999999999</v>
       </c>
-      <c r="E11">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>214.75199999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C12">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D12">
-        <v>0.1</v>
-      </c>
-      <c r="E12">
-        <v>0.33</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>5.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10.2829727759042</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="D13">
         <v>427.68</v>
-      </c>
-      <c r="E13">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>429.56900000000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>53.41</v>
@@ -4789,7 +4613,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B28">
         <v>4.1500000000000004</v>
@@ -4804,441 +4628,587 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="63.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="47" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>9.9110603332499994E-4</v>
+      </c>
+      <c r="D2">
+        <v>8.4090232849099995E-4</v>
+      </c>
+      <c r="E2">
+        <f>C2-D2</f>
+        <v>1.5020370483399999E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0.22456908226</v>
+      </c>
+      <c r="D3">
+        <v>2.72607803345E-3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E6" si="0">C3-D3</f>
+        <v>0.22184300422654998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>6.9360017776499999E-2</v>
+      </c>
+      <c r="D4">
+        <v>3.77106666565E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>6.5588951110850002E-2</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>5.5372953414899999E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.25019454956E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5.312275886534E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="5"/>
-      <c r="C7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="6" t="e">
+      <c r="C6">
+        <v>7.4239015579199999E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.88145446777E-4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>7.3850870132423002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5">
+        <f>AVERAGE(C2:C6)</f>
+        <v>8.4906435012784998E-2</v>
+      </c>
+      <c r="D7" s="5">
         <f>AVERAGE(D2:D6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E7" s="6" t="e">
+        <v>1.9952774047856002E-3</v>
+      </c>
+      <c r="E7" s="5">
         <f>AVERAGE(E2:E6)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="6" t="e">
-        <f>AVERAGE(F2:F6)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.2911157607999414E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8">
-        <f>D8-E8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>4.0800571441700004E-3</v>
+      </c>
+      <c r="D8">
+        <v>7.0469379425000004E-3</v>
+      </c>
+      <c r="E8">
+        <f>C8-D8</f>
+        <v>-2.9668807983300001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="F9">
-        <f t="shared" ref="F3:F30" si="0">D9-E9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="10">
+        <v>0.33794879913300002</v>
+      </c>
+      <c r="D9">
+        <v>4.80794906616E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E30" si="1">C9-D9</f>
+        <v>0.33314085006684002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>8.8738203048700004E-2</v>
+      </c>
+      <c r="D10">
+        <v>6.9618225097699998E-4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>8.8042020797722997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.43239092826800002</v>
+      </c>
+      <c r="D11">
+        <v>1.0440111160299999E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.42195081710769999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A13" s="5"/>
-      <c r="C13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="6" t="e">
+      <c r="C12">
+        <v>0.193861961365</v>
+      </c>
+      <c r="D12">
+        <v>2.54797935486E-3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.19131398201013999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="5">
+        <f>AVERAGE(C8:C12)</f>
+        <v>0.21140398979177402</v>
+      </c>
+      <c r="D13" s="5">
         <f>AVERAGE(D8:D12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="6" t="e">
+        <v>5.1078319549594008E-3</v>
+      </c>
+      <c r="E13" s="5">
         <f>AVERAGE(E8:E12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="6">
-        <f>AVERAGE(F8:F12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.2062961578368146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>5.8948993682900004E-3</v>
+      </c>
+      <c r="D14">
+        <v>1.7518997192399999E-3</v>
+      </c>
+      <c r="E14">
+        <f>C14-D14</f>
+        <v>4.1429996490500009E-3</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.27640199661300002</v>
+      </c>
+      <c r="D15">
+        <v>5.6059360504200004E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ref="E15:E18" si="2">C15-D15</f>
+        <v>0.27079606056258004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3.78139019012E-2</v>
+      </c>
+      <c r="D16">
+        <v>1.54209136963E-3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>3.6271810531569998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>4.7414064407299998E-2</v>
+      </c>
+      <c r="D17">
+        <v>6.1869621276899999E-3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>4.1227102279609996E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="C19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="6" t="e">
+      <c r="C18">
+        <v>8.2016944885299994E-2</v>
+      </c>
+      <c r="D18">
+        <v>5.4299831390400002E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>7.6586961746259993E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5">
+        <f>AVERAGE(C14:C18)</f>
+        <v>8.9908361435018E-2</v>
+      </c>
+      <c r="D19" s="5">
         <f>AVERAGE(D14:D18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="6" t="e">
+        <v>4.1033744812040002E-3</v>
+      </c>
+      <c r="E19" s="5">
         <f>AVERAGE(E14:E18)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F19" s="6" t="e">
-        <f>AVERAGE(F14:F18)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8.5804986953814028E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2.0039081573500002E-3</v>
+      </c>
+      <c r="D20">
+        <v>5.3215026855499997E-4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1.4717578887950002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="10">
+        <v>2.0617940425899999</v>
+      </c>
+      <c r="D21">
+        <v>4.0540695190399998E-3</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>2.05773997307096</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0.140160083771</v>
+      </c>
+      <c r="D22">
+        <v>2.64000892639E-3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.13752007484461001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>6</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="10">
+        <v>0.169538974762</v>
+      </c>
+      <c r="D23">
+        <v>8.5110664367699998E-3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0.16102790832523001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
-      <c r="C25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="6" t="e">
+      <c r="C24">
+        <v>5.9026956558199999E-2</v>
+      </c>
+      <c r="D24">
+        <v>3.8700103759799999E-3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>5.5156946182220001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5">
+        <f>AVERAGE(C20:C24)</f>
+        <v>0.48650479316771006</v>
+      </c>
+      <c r="D25" s="5">
         <f>AVERAGE(D20:D24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="6" t="e">
+        <v>3.9214611053469996E-3</v>
+      </c>
+      <c r="E25" s="5">
         <f>AVERAGE(E20:E24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F25" s="6">
-        <f>AVERAGE(F20:F24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.48258333206236292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
-        <v>65</v>
+      <c r="C26">
+        <v>0.14033198356599999</v>
       </c>
       <c r="D26">
-        <v>0.47318601608299998</v>
+        <v>6.1030387878399997E-3</v>
       </c>
       <c r="E26">
-        <v>1.6916990280199998E-2</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>0.45626902580279999</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>39</v>
-      </c>
-      <c r="I26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.13422894477816</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>7</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>0.139679193497</v>
+      </c>
+      <c r="D27">
+        <v>9.9158287048299997E-3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.12976336479217002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>7</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="10">
+        <v>3.07358598709</v>
+      </c>
+      <c r="D28">
+        <v>9.1910362243699997E-3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>3.0643949508656299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>7</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>3.1640052795399998E-2</v>
+      </c>
+      <c r="D29">
+        <v>8.85009765625E-4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>3.0755043029774998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>7</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A31" s="5"/>
-      <c r="C31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="C30">
+        <v>0.33597898483299998</v>
+      </c>
+      <c r="D30">
+        <v>1.6850948333699999E-2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.31912803649929999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5">
+        <f>AVERAGE(C26:C30)</f>
+        <v>0.74424324035627998</v>
+      </c>
+      <c r="D31" s="5">
         <f>AVERAGE(D26:D30)</f>
-        <v>0.47318601608299998</v>
-      </c>
-      <c r="E31" s="6">
+        <v>8.589172363273001E-3</v>
+      </c>
+      <c r="E31" s="5">
         <f>AVERAGE(E26:E30)</f>
-        <v>1.6916990280199998E-2</v>
-      </c>
-      <c r="F31" s="6">
-        <f>AVERAGE(F26:F30)</f>
-        <v>9.1253805160560003E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="F32" s="6" t="e">
-        <f>AVERAGE(F7,F13,F19,F25,F31)</f>
-        <v>#DIV/0!</v>
+        <v>0.73565406799300703</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E32" s="5">
+        <f>AVERAGE(E7,E13,E19,E25,E31)</f>
+        <v>0.31864994049079959</v>
       </c>
     </row>
   </sheetData>
@@ -5268,19 +5238,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5289,184 +5259,184 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>49</v>
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5493,19 +5463,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5514,184 +5484,184 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>49</v>
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5718,210 +5688,210 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>49</v>
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5950,25 +5920,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
       <c r="I1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5976,191 +5946,191 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I2">
         <v>0.22014403343200001</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>49</v>
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6171,8 +6141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6187,301 +6157,301 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1.22451903405899E-5</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1.30730858148743E-5</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="9">
+        <v>5.1931818181818101E-6</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="9">
+        <v>5.4721664168040596E-6</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="9">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1.20452448760635E-5</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="9">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1.8452363336314102E-5</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1.7359516528926399E-5</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1.9402476155750199E-5</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="9">
+        <v>2.54689697393084E-5</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1.2370595785032599E-8</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="9">
+        <v>5.4721664168040596E-6</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1.8452363336314102E-5</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="B20" s="9">
+        <v>7.8582170342663692E-6</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="10">
-        <v>1.22451903405899E-5</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B21" s="9">
+        <v>5.1241264671323601E-5</v>
+      </c>
+      <c r="C21" s="9">
+        <v>5.5544105523551599E-7</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="10">
-        <v>1.30730858148743E-5</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="10">
-        <v>5.1931818181818101E-6</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="B22" s="9">
+        <v>5.43748836873962E-6</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="10">
-        <v>5.4721664168040596E-6</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B23" s="9">
+        <v>5.1469215394822304E-6</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="10">
-        <v>7.8582170342663692E-6</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="B24" s="9">
+        <v>4.3494635989035301E-5</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1.20476216749328E-6</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="10">
-        <v>1.20452448760635E-5</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="B25" s="9">
+        <v>9.0625332665379805E-6</v>
+      </c>
+      <c r="C25" s="9">
+        <v>5.4873559636968102E-8</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="10">
-        <v>7.8582170342663692E-6</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="10">
-        <v>1.8452363336314102E-5</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="10">
-        <v>1.7359516528926399E-5</v>
-      </c>
-      <c r="C15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="10">
-        <v>1.9402476155750199E-5</v>
-      </c>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="10">
-        <v>2.54689697393084E-5</v>
-      </c>
-      <c r="C17" s="10">
-        <v>1.2370595785032599E-8</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="10">
-        <v>5.4721664168040596E-6</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B19" s="10">
-        <v>1.8452363336314102E-5</v>
-      </c>
-      <c r="C19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B20" s="10">
-        <v>7.8582170342663692E-6</v>
-      </c>
-      <c r="C20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="10">
-        <v>5.1241264671323601E-5</v>
-      </c>
-      <c r="C21" s="10">
-        <v>5.5544105523551599E-7</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="10">
-        <v>5.43748836873962E-6</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="10">
-        <v>5.1469215394822304E-6</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="10">
-        <v>4.3494635989035301E-5</v>
-      </c>
-      <c r="C24" s="10">
-        <v>1.20476216749328E-6</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" s="10">
-        <v>9.0625332665379805E-6</v>
-      </c>
-      <c r="C25" s="10">
-        <v>5.4873559636968102E-8</v>
-      </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="10">
+      <c r="B26" s="9">
         <v>8.3622676310891896E-6</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="9">
         <v>1.04063454274664E-7</v>
       </c>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated Images and tested improved HITS
</commit_message>
<xml_diff>
--- a/Risultati/Risultati Search Engine.xlsx
+++ b/Risultati/Risultati Search Engine.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
   <si>
     <t>HITS</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>http://www.ign.com/articles/2014/06/05/earthnight-coming-to-ps4-ps-vita</t>
+  </si>
+  <si>
+    <t>HITS improved</t>
   </si>
 </sst>
 </file>
@@ -401,15 +404,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tempi</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> esecuzione </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Pagerank</a:t>
+              <a:t>Pagerank Execution Times</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -544,11 +539,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="305274416"/>
-        <c:axId val="140539000"/>
+        <c:axId val="312377032"/>
+        <c:axId val="312377416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="305274416"/>
+        <c:axId val="312377032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -590,7 +585,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140539000"/>
+        <c:crossAx val="312377416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,7 +593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140539000"/>
+        <c:axId val="312377416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +643,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="305274416"/>
+        <c:crossAx val="312377032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -749,7 +744,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tempi esecuzione HITS</a:t>
+              <a:t>HITS Execution Times</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -797,15 +792,72 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>HITS Improved</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>(Ranking!$C$14,Ranking!$C$14,Ranking!$C$14,Ranking!$C$14,Ranking!$C$14,Ranking!$C$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116.224257655071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>HITS</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -884,11 +936,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="140542136"/>
-        <c:axId val="140540176"/>
+        <c:axId val="311314688"/>
+        <c:axId val="311313512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140542136"/>
+        <c:axId val="311314688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -930,7 +982,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140540176"/>
+        <c:crossAx val="311313512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -938,7 +990,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140540176"/>
+        <c:axId val="311313512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -988,7 +1040,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140542136"/>
+        <c:crossAx val="311314688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1000,6 +1052,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1094,7 +1177,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1269,11 +1351,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="140543704"/>
-        <c:axId val="140541352"/>
+        <c:axId val="312489352"/>
+        <c:axId val="312491312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140543704"/>
+        <c:axId val="312489352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1315,7 +1397,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140541352"/>
+        <c:crossAx val="312491312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1323,7 +1405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140541352"/>
+        <c:axId val="312491312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1373,7 +1455,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140543704"/>
+        <c:crossAx val="312489352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1387,7 +1469,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1515,7 +1596,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1712,11 +1792,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="140537824"/>
-        <c:axId val="140540568"/>
+        <c:axId val="312492488"/>
+        <c:axId val="312494056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140537824"/>
+        <c:axId val="312492488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1758,7 +1838,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140540568"/>
+        <c:crossAx val="312494056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1766,7 +1846,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140540568"/>
+        <c:axId val="312494056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +1896,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140537824"/>
+        <c:crossAx val="312492488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,7 +1918,6 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4446,8 +4525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,6 +4670,17 @@
       </c>
       <c r="C13">
         <v>427.68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14">
+        <v>116.224257655071</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>